<commit_message>
Master Template files are added
</commit_message>
<xml_diff>
--- a/src/main/resources/Dock.xlsx
+++ b/src/main/resources/Dock.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9024" firstSheet="1"/>
+    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Dock ID</t>
   </si>
@@ -30,47 +43,11 @@
   <si>
     <t>Store ID</t>
   </si>
-  <si>
-    <t>RM Dock 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oversize Material </t>
-  </si>
-  <si>
-    <t>pratik@aceme.net</t>
-  </si>
-  <si>
-    <t>RM Dock 2</t>
-  </si>
-  <si>
-    <t>Pallets &amp; Cartons</t>
-  </si>
-  <si>
-    <t>yash@aceme.net</t>
-  </si>
-  <si>
-    <t>RM Dock 3</t>
-  </si>
-  <si>
-    <t>Tanks, Drums, etc.</t>
-  </si>
-  <si>
-    <t>nitin@aceme.net</t>
-  </si>
-  <si>
-    <t>RM Dock 4</t>
-  </si>
-  <si>
-    <t>Rejected Material</t>
-  </si>
-  <si>
-    <t>vishal@aceme.net</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -866,7 +843,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1180,14 +1157,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="$A2:$XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="22.287037037037" customWidth="1"/>
-    <col min="4" max="4" width="26.287037037037" customWidth="1"/>
+    <col min="2" max="3" width="22.29" customWidth="1"/>
+    <col min="4" max="4" width="26.29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1207,73 +1184,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="13.2" spans="1:5">
+    <row r="2" ht="12.5" spans="1:5">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9">
-        <v>1</v>
-      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
-    <row r="3" ht="13.2" spans="1:5">
+    <row r="3" ht="12.5" spans="1:5">
       <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="12">
-        <v>6</v>
-      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
     </row>
-    <row r="4" ht="13.2" spans="1:5">
+    <row r="4" ht="12.5" spans="1:5">
       <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="12">
-        <v>4</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
     </row>
-    <row r="5" ht="13.2" spans="1:5">
+    <row r="5" ht="12.5" spans="1:5">
       <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="12">
-        <v>5</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="pratik@aceme.net"/>
-    <hyperlink ref="D3" r:id="rId2" display="yash@aceme.net"/>
-    <hyperlink ref="D4" r:id="rId3" display="nitin@aceme.net"/>
-    <hyperlink ref="D5" r:id="rId4" display="vishal@aceme.net"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>